<commit_message>
Actualizacion de formulas mat 8 T1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion11/ESCALETA_MA_07_11_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion11/ESCALETA_MA_07_11_CO.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -961,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1085,6 +1085,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1393,9 +1396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2731,7 +2734,7 @@
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="49" t="s">
         <v>189</v>
       </c>
       <c r="H24" s="3">

</xml_diff>